<commit_message>
Add HEX tester to Excel file
</commit_message>
<xml_diff>
--- a/documents/ISA.xlsx
+++ b/documents/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naoya\OneDrive\ドキュメント\慶應義塾大学大学院\計算機システム設計論\compsys2018-6\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{80C438F1-E5FD-4156-8A30-8ED91F7346A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E5376EE0-F862-41B1-BE12-5729E0B1DD5C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="命令" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
   <si>
     <t>背景灰色は実装しない</t>
   </si>
@@ -344,6 +344,62 @@
   </si>
   <si>
     <t>base</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32bit読み込み</t>
+    <rPh sb="5" eb="6">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32bit書き込み</t>
+    <rPh sb="5" eb="6">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8bit読み取り</t>
+    <rPh sb="4" eb="5">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8bit書き込み</t>
+    <rPh sb="4" eb="5">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>lb rt,base,offset</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sb rt,base,offset</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rt=dmem(base+offset)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>dmem(base+offset)=rt</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -452,9 +508,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -463,6 +516,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -850,7 +906,7 @@
   <dimension ref="A1:AL26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -871,7 +927,7 @@
       <c r="E1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G1" t="str">
@@ -902,7 +958,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N1" s="7" t="str">
+      <c r="N1" s="6" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -934,7 +990,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V1" s="7" t="str">
+      <c r="V1" s="6" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -966,7 +1022,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD1" s="7" t="str">
+      <c r="AD1" s="6" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -998,7 +1054,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AL1" s="7" t="str">
+      <c r="AL1" s="6" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1007,11 +1063,11 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AL2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AL2" s="6"/>
     </row>
     <row r="3" spans="1:38" ht="18.75" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1029,7 +1085,7 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2">
         <v>31</v>
       </c>
@@ -1051,7 +1107,7 @@
       <c r="M3" s="2">
         <v>25</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>24</v>
       </c>
       <c r="O3" s="2">
@@ -1075,7 +1131,7 @@
       <c r="U3" s="2">
         <v>17</v>
       </c>
-      <c r="V3" s="8">
+      <c r="V3" s="7">
         <v>16</v>
       </c>
       <c r="W3" s="2">
@@ -1099,7 +1155,7 @@
       <c r="AC3" s="2">
         <v>9</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AD3" s="7">
         <v>8</v>
       </c>
       <c r="AE3" s="2">
@@ -1123,7 +1179,7 @@
       <c r="AK3" s="2">
         <v>1</v>
       </c>
-      <c r="AL3" s="8">
+      <c r="AL3" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1161,34 +1217,34 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6" t="s">
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6" t="s">
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
       <c r="AG4">
         <v>1</v>
       </c>
@@ -1242,34 +1298,34 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6" t="s">
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6" t="s">
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
       <c r="AG5">
         <v>1</v>
       </c>
@@ -1323,34 +1379,34 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6" t="s">
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6" t="s">
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
       <c r="AG6">
         <v>1</v>
       </c>
@@ -1404,34 +1460,34 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6" t="s">
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6" t="s">
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
       <c r="AG7">
         <v>0</v>
       </c>
@@ -1485,34 +1541,34 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6" t="s">
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6" t="s">
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6" t="s">
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
       <c r="AG8">
         <v>1</v>
       </c>
@@ -1566,34 +1622,34 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6" t="s">
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6" t="s">
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
       <c r="AG9">
         <v>1</v>
       </c>
@@ -1647,34 +1703,34 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6" t="s">
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6" t="s">
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6" t="s">
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
       <c r="AG10">
         <v>1</v>
       </c>
@@ -1728,13 +1784,13 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="5">
         <v>0</v>
       </c>
@@ -1765,13 +1821,13 @@
       <c r="AA11" s="5">
         <v>0</v>
       </c>
-      <c r="AB11" s="6" t="s">
+      <c r="AB11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
       <c r="AG11">
         <v>0</v>
       </c>
@@ -1819,13 +1875,13 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="5">
         <v>0</v>
       </c>
@@ -1856,13 +1912,13 @@
       <c r="AA12" s="5">
         <v>0</v>
       </c>
-      <c r="AB12" s="6" t="s">
+      <c r="AB12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
       <c r="AG12">
         <v>0</v>
       </c>
@@ -1913,38 +1969,38 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6" t="s">
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6" t="s">
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
-      <c r="AL13" s="6"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
     </row>
     <row r="14" spans="1:38" ht="18.75" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -1974,38 +2030,38 @@
       <c r="L14">
         <v>1</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6" t="s">
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="6"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
     </row>
     <row r="15" spans="1:38" ht="18.75" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -2038,38 +2094,38 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6" t="s">
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6" t="s">
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-      <c r="AI15" s="6"/>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" s="6"/>
-      <c r="AL15" s="6"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="9"/>
     </row>
     <row r="16" spans="1:38" ht="18.75" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -2111,31 +2167,31 @@
       <c r="Q16" s="5">
         <v>0</v>
       </c>
-      <c r="R16" s="6" t="s">
+      <c r="R16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6" t="s">
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="6"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
     </row>
     <row r="17" spans="1:38" ht="18.75" customHeight="1">
       <c r="A17" s="1" t="s">
@@ -2168,38 +2224,38 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6" t="s">
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6" t="s">
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
-      <c r="AG17" s="6"/>
-      <c r="AH17" s="6"/>
-      <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="6"/>
-      <c r="AL17" s="6"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
     </row>
     <row r="18" spans="1:38" ht="18.75" customHeight="1">
       <c r="A18" s="1" t="s">
@@ -2232,38 +2288,38 @@
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6" t="s">
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6" t="s">
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
-      <c r="AG18" s="6"/>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="6"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="9"/>
     </row>
     <row r="19" spans="1:38" ht="18.75" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -2296,34 +2352,34 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="6"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
     </row>
     <row r="20" spans="1:38" ht="18.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -2356,34 +2412,34 @@
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
-      <c r="AL20" s="6"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
     </row>
     <row r="21" spans="1:38" ht="18.75" customHeight="1">
       <c r="A21" s="1" t="s">
@@ -2392,6 +2448,15 @@
       <c r="B21" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="G21">
         <v>1</v>
       </c>
@@ -2410,38 +2475,38 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6" t="s">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6" t="s">
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="6"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
     </row>
     <row r="22" spans="1:38" ht="18.75" customHeight="1">
       <c r="A22" s="1" t="s">
@@ -2450,6 +2515,15 @@
       <c r="B22" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="G22">
         <v>1</v>
       </c>
@@ -2468,38 +2542,38 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6" t="s">
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6" t="s">
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="6"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
     </row>
     <row r="23" spans="1:38" ht="18.75" customHeight="1">
       <c r="A23" s="1" t="s">
@@ -2508,6 +2582,9 @@
       <c r="B23" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
@@ -2529,38 +2606,38 @@
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6" t="s">
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6" t="s">
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="6"/>
-      <c r="AG23" s="6"/>
-      <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="6"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
     </row>
     <row r="24" spans="1:38" ht="18.75" customHeight="1">
       <c r="A24" s="1" t="s">
@@ -2569,6 +2646,9 @@
       <c r="B24" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>85</v>
       </c>
@@ -2590,82 +2670,59 @@
       <c r="L24">
         <v>1</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6" t="s">
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6" t="s">
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
-      <c r="AL24" s="6"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="9"/>
+      <c r="AL24" s="9"/>
     </row>
     <row r="25" spans="1:38" ht="18.75" customHeight="1"/>
     <row r="26" spans="1:38" ht="18.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="R23:V23"/>
-    <mergeCell ref="W23:AL23"/>
-    <mergeCell ref="M24:Q24"/>
-    <mergeCell ref="R24:V24"/>
-    <mergeCell ref="W24:AL24"/>
-    <mergeCell ref="M21:Q21"/>
-    <mergeCell ref="R21:V21"/>
-    <mergeCell ref="W21:AL21"/>
-    <mergeCell ref="M22:Q22"/>
-    <mergeCell ref="R22:V22"/>
-    <mergeCell ref="W22:AL22"/>
-    <mergeCell ref="M18:Q18"/>
-    <mergeCell ref="R18:V18"/>
-    <mergeCell ref="W18:AL18"/>
-    <mergeCell ref="M19:AL19"/>
-    <mergeCell ref="M20:AL20"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="W16:AL16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="R17:V17"/>
-    <mergeCell ref="W17:AL17"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="R14:V14"/>
-    <mergeCell ref="W14:AL14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="R15:V15"/>
-    <mergeCell ref="W15:AL15"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="AB12:AF12"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="R13:V13"/>
-    <mergeCell ref="W13:AL13"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="W10:AA10"/>
-    <mergeCell ref="AB10:AF10"/>
-    <mergeCell ref="M11:Q11"/>
-    <mergeCell ref="AB11:AF11"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="W4:AA4"/>
+    <mergeCell ref="AB4:AF4"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R5:V5"/>
+    <mergeCell ref="W5:AA5"/>
+    <mergeCell ref="AB5:AF5"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="W6:AA6"/>
+    <mergeCell ref="AB6:AF6"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
     <mergeCell ref="M8:Q8"/>
     <mergeCell ref="R8:V8"/>
     <mergeCell ref="W8:AA8"/>
@@ -2674,22 +2731,45 @@
     <mergeCell ref="R9:V9"/>
     <mergeCell ref="W9:AA9"/>
     <mergeCell ref="AB9:AF9"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="R6:V6"/>
-    <mergeCell ref="W6:AA6"/>
-    <mergeCell ref="AB6:AF6"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="W4:AA4"/>
-    <mergeCell ref="AB4:AF4"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="R5:V5"/>
-    <mergeCell ref="W5:AA5"/>
-    <mergeCell ref="AB5:AF5"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="W10:AA10"/>
+    <mergeCell ref="AB10:AF10"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="AB11:AF11"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="AB12:AF12"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="R13:V13"/>
+    <mergeCell ref="W13:AL13"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="W14:AL14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="R15:V15"/>
+    <mergeCell ref="W15:AL15"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="W16:AL16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="R17:V17"/>
+    <mergeCell ref="W17:AL17"/>
+    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="R18:V18"/>
+    <mergeCell ref="W18:AL18"/>
+    <mergeCell ref="M19:AL19"/>
+    <mergeCell ref="M20:AL20"/>
+    <mergeCell ref="M21:Q21"/>
+    <mergeCell ref="R21:V21"/>
+    <mergeCell ref="W21:AL21"/>
+    <mergeCell ref="M22:Q22"/>
+    <mergeCell ref="R22:V22"/>
+    <mergeCell ref="W22:AL22"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="R23:V23"/>
+    <mergeCell ref="W23:AL23"/>
+    <mergeCell ref="M24:Q24"/>
+    <mergeCell ref="R24:V24"/>
+    <mergeCell ref="W24:AL24"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add rand instruction (not implemented yet)
</commit_message>
<xml_diff>
--- a/documents/ISA.xlsx
+++ b/documents/ISA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="116">
   <si>
     <t xml:space="preserve">背景灰色は実装しない</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t xml:space="preserve">pop rs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rs=rand()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand rs</t>
   </si>
   <si>
     <t xml:space="preserve">lb</t>
@@ -611,10 +620,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL32"/>
+  <dimension ref="A1:AL33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO10" activeCellId="0" sqref="AO10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2603,22 +2612,19 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="G26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>0</v>
@@ -2633,77 +2639,115 @@
         <v>0</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-      <c r="R26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="6"/>
-      <c r="AF26" s="6"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-      <c r="AI26" s="6"/>
-      <c r="AJ26" s="6"/>
-      <c r="AK26" s="6"/>
-      <c r="AL26" s="6"/>
+      <c r="R26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="E27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="G27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -2740,9 +2784,12 @@
         <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -2755,19 +2802,19 @@
         <v>0</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -2819,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0</v>
@@ -2831,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -2863,48 +2910,112 @@
       <c r="AK29" s="6"/>
       <c r="AL29" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F31" s="0" t="s">
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AH30" s="6"/>
+      <c r="AI30" s="6"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="6"/>
+      <c r="AL30" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="71">
     <mergeCell ref="M4:Q4"/>
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="W4:AA4"/>
@@ -2964,8 +3075,6 @@
     <mergeCell ref="M24:Q24"/>
     <mergeCell ref="M25:Q25"/>
     <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="R26:V26"/>
-    <mergeCell ref="W26:AL26"/>
     <mergeCell ref="M27:Q27"/>
     <mergeCell ref="R27:V27"/>
     <mergeCell ref="W27:AL27"/>
@@ -2975,6 +3084,9 @@
     <mergeCell ref="M29:Q29"/>
     <mergeCell ref="R29:V29"/>
     <mergeCell ref="W29:AL29"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="R30:V30"/>
+    <mergeCell ref="W30:AL30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3006,13 +3118,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -3031,7 +3143,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -3042,7 +3154,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -3053,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -3064,7 +3176,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -3075,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -3086,7 +3198,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -3097,7 +3209,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -3108,7 +3220,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3119,7 +3231,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3130,7 +3242,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -3141,7 +3253,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -3152,7 +3264,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -3163,7 +3275,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -3174,7 +3286,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -3185,7 +3297,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1023</v>
@@ -3196,7 +3308,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -3207,7 +3319,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -3218,7 +3330,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -3229,7 +3341,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -3240,7 +3352,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0</v>
@@ -3251,7 +3363,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0</v>
@@ -3262,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0</v>
@@ -3273,7 +3385,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0</v>
@@ -3284,7 +3396,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
@@ -3295,7 +3407,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>0</v>
@@ -3306,7 +3418,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0</v>
@@ -3317,7 +3429,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>0</v>
@@ -3328,7 +3440,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
@@ -3339,7 +3451,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0</v>
@@ -3350,7 +3462,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
@@ -3361,7 +3473,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>

</xml_diff>